<commit_message>
Many updates to allow AEAS importing
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://readingschoolco-my.sharepoint.com/personal/adimmick_reading-school_co_uk/Documents/Projects/ReportWriter/app/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{8FC2F979-F691-264D-BF03-F049BC0D1611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1177685-35FA-4947-A6F4-9B6FCCA9AB63}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{8FC2F979-F691-264D-BF03-F049BC0D1611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66822189-559A-244F-8619-8278F2DA0979}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
+    <workbookView xWindow="5640" yWindow="2360" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
     <sheet name="Data entry" sheetId="1" r:id="rId2"/>
     <sheet name="Comment bank" sheetId="2" r:id="rId3"/>
-    <sheet name="Info" sheetId="3" r:id="rId4"/>
+    <sheet name="Info" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Metadata" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>ReportWriter</t>
   </si>
@@ -113,12 +114,27 @@
   <si>
     <t>Category</t>
   </si>
+  <si>
+    <t>This report contains data that is required for ReportWriter to function correctly. Do not change any values in this sheet!</t>
+  </si>
+  <si>
+    <t>Report ID</t>
+  </si>
+  <si>
+    <t>Raw text</t>
+  </si>
+  <si>
+    <t>Compiled report</t>
+  </si>
+  <si>
+    <t>Complete status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +171,21 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -317,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -341,6 +372,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -350,13 +389,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B44B346-320A-5B41-8D50-F9DF55326F83}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -710,15 +743,15 @@
       </c>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:10" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="15" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -769,15 +802,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA002F8-9FB7-404F-989E-62085E85C1B3}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="87.1640625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="35" style="20" customWidth="1"/>
+    <col min="2" max="2" width="87.1640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="35" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
@@ -796,7 +829,7 @@
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -816,7 +849,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,4 +875,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D7FC91-FF52-B54F-AE06-0630AB43EF60}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added gender-specific pronoun support. This will break compatibility with previous report set documents.
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://readingschoolco-my.sharepoint.com/personal/adimmick_reading-school_co_uk/Documents/Projects/ReportWriter/app/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad\PycharmProjects\ReportWriter\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{8FC2F979-F691-264D-BF03-F049BC0D1611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66822189-559A-244F-8619-8278F2DA0979}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1632F8F4-FECB-411F-B7C5-DEB9F2E7317E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="2360" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>ReportWriter</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Complete status</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -380,6 +383,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -389,7 +393,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +408,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -712,7 +711,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -720,42 +719,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B44B346-320A-5B41-8D50-F9DF55326F83}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="46.83203125" style="13" customWidth="1"/>
-    <col min="7" max="10" width="14" customWidth="1"/>
+    <col min="1" max="1" width="16.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="31.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.375" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="46.875" style="13" customWidth="1"/>
+    <col min="8" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:10" s="19" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" s="20" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -763,35 +763,38 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:XFD2"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:XFD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -806,26 +809,26 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="87.1640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="87.125" style="16" customWidth="1"/>
     <col min="3" max="3" width="35" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:3" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
@@ -836,7 +839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
     </row>
   </sheetData>
@@ -852,19 +855,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -885,29 +888,29 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the ReportWriter template and layout.html to change references to "data labels" to "perspective labels"
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad\PycharmProjects\ReportWriter\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1632F8F4-FECB-411F-B7C5-DEB9F2E7317E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C57FEA-2C81-40AE-9347-C8BDEBA93A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
+    <workbookView xWindow="4710" yWindow="1095" windowWidth="18240" windowHeight="11160" activeTab="1" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -81,8 +81,44 @@
     <t>Label4</t>
   </si>
   <si>
+    <t>Data entry template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version </t>
+  </si>
+  <si>
+    <t>Comment bank</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>This report contains data that is required for ReportWriter to function correctly. Do not change any values in this sheet!</t>
+  </si>
+  <si>
+    <t>Report ID</t>
+  </si>
+  <si>
+    <t>Raw text</t>
+  </si>
+  <si>
+    <t>Compiled report</t>
+  </si>
+  <si>
+    <t>Complete status</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Data values </t>
+      <t xml:space="preserve">Report Perspective data values </t>
     </r>
     <r>
       <rPr>
@@ -95,42 +131,6 @@
       </rPr>
       <t>(add as many additional data value columns as required)</t>
     </r>
-  </si>
-  <si>
-    <t>Data entry template</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version </t>
-  </si>
-  <si>
-    <t>Comment bank</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>This report contains data that is required for ReportWriter to function correctly. Do not change any values in this sheet!</t>
-  </si>
-  <si>
-    <t>Report ID</t>
-  </si>
-  <si>
-    <t>Raw text</t>
-  </si>
-  <si>
-    <t>Compiled report</t>
-  </si>
-  <si>
-    <t>Complete status</t>
-  </si>
-  <si>
-    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -752,7 +752,7 @@
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="21" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>4</v>
@@ -824,19 +824,19 @@
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -864,12 +864,12 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -897,21 +897,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed edit/add comment bug. Added userguide link to front page. Updated template to include instructions.
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://readingschoolco-my.sharepoint.com/personal/adimmick_reading-school_co_uk/Documents/Projects/ReportWriter/app/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C57FEA-2C81-40AE-9347-C8BDEBA93A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{37C57FEA-2C81-40AE-9347-C8BDEBA93A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E8F472C-894C-FC42-AF8E-0C8F798D5B32}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="1095" windowWidth="18240" windowHeight="11160" activeTab="1" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
+    <workbookView xWindow="9340" yWindow="6540" windowWidth="23340" windowHeight="14920" xr2:uid="{DE9C204F-D06B-8549-8CED-AA5B34033AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>ReportWriter</t>
   </si>
@@ -118,7 +118,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Report Perspective data values </t>
+      <t xml:space="preserve">Student data values </t>
     </r>
     <r>
       <rPr>
@@ -132,12 +132,76 @@
       <t>(add as many additional data value columns as required)</t>
     </r>
   </si>
+  <si>
+    <t>This is a ReportWriter template, designed for use with the online ReportWriter app.</t>
+  </si>
+  <si>
+    <t>Open the ReportWriter webapp!</t>
+  </si>
+  <si>
+    <t>Using this template</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To get started writing reports, simply add details about your students into the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Data entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab, including any data that you wish to refer to and include in your reports. You can also add (or reuse) comment bank comments by writing them in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Comment bank </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tab.
+Once you have added your student details and data you can upload this template file to the ReportWriter web app, where you will be able to use its rich functionality to help you write insightful, individual, data-driven reports.
+If you need any additional help using ReportWriter, please consult the User Guide.</t>
+    </r>
+  </si>
+  <si>
+    <t>Open the ReportWriter User Guide</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,8 +253,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +287,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -348,10 +438,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -393,8 +484,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -707,43 +812,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDAE958-D5A5-8A4E-960A-E10087054F2F}">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor theme="3" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="11" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" s="29" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="8" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="136" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A10:K10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{6D6B7F56-5583-D64F-84E3-44FC1A74B2A1}"/>
+    <hyperlink ref="B11" r:id="rId2" display="Open the ReportWrtier User Guide" xr:uid="{634094F6-0812-9A44-BC26-113C5AEB4A9D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B44B346-320A-5B41-8D50-F9DF55326F83}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="9.25" customWidth="1"/>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="31.5" style="3" customWidth="1"/>
-    <col min="6" max="6" width="24.375" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="46.875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="46.83203125" style="13" customWidth="1"/>
     <col min="8" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:11" s="20" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="20" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
@@ -755,7 +932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -803,32 +980,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA002F8-9FB7-404F-989E-62085E85C1B3}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="87.125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="87.1640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="35" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -839,7 +1019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
     </row>
   </sheetData>
@@ -855,19 +1035,19 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -888,19 +1068,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>20</v>
       </c>

</xml_diff>